<commit_message>
Update GA2.3 answer URL for correct resource access
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
   <si>
     <t>TASK</t>
   </si>
@@ -245,13 +245,16 @@
     <t>What is the GitHub Pages URL</t>
   </si>
   <si>
-    <t>https://telvinvarghese.github.io/website/?v=1</t>
+    <t>https://tusharisme.github.io/tds_work</t>
   </si>
   <si>
     <t>GA2.4</t>
   </si>
   <si>
     <t>Run this program on Google Colab</t>
+  </si>
+  <si>
+    <t>013af</t>
   </si>
   <si>
     <t>GA2.5</t>
@@ -1335,16 +1338,16 @@
       <c r="B23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="7">
-        <v>22557</v>
+      <c r="C23" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C24" s="7">
         <v>6378</v>
@@ -1352,76 +1355,76 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C31" s="7">
         <v>47</v>
@@ -1429,87 +1432,87 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C39" s="7">
         <v>260</v>
@@ -1517,43 +1520,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C43" s="9">
         <v>10.1399458</v>
@@ -1561,43 +1564,43 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C47" s="7">
         <v>29658</v>
@@ -1605,21 +1608,21 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C49" s="9">
         <v>0.475186494865336</v>
@@ -1627,10 +1630,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C50" s="7">
         <v>22</v>
@@ -1638,10 +1641,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C51" s="7">
         <v>173</v>
@@ -1649,10 +1652,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C52" s="7">
         <v>10930</v>
@@ -1660,10 +1663,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C53" s="7">
         <v>10829</v>
@@ -1671,10 +1674,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C54" s="7">
         <v>53117</v>
@@ -1682,10 +1685,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C55" s="7">
         <v>27925</v>
@@ -1693,32 +1696,32 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>55</v>

</xml_diff>